<commit_message>
impprove tags function, sessions section and responsiveness
</commit_message>
<xml_diff>
--- a/Server/public/sessions/004243/attendees.xlsx
+++ b/Server/public/sessions/004243/attendees.xlsx
@@ -427,7 +427,7 @@
         <v>21BCS079</v>
       </c>
       <c r="C2" t="str">
-        <v>A</v>
+        <v>P</v>
       </c>
       <c r="D2" t="str">
         <v xml:space="preserve"> </v>
@@ -441,7 +441,7 @@
         <v>21BCS080</v>
       </c>
       <c r="C3" t="str">
-        <v>A</v>
+        <v>P</v>
       </c>
       <c r="D3" t="str">
         <v xml:space="preserve"> </v>

</xml_diff>